<commit_message>
Excel data is updated by Mayank
</commit_message>
<xml_diff>
--- a/gitwa excelwa.xlsx
+++ b/gitwa excelwa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash.b.dwivedi\Documents\gitwa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Practice\Test_Repo_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F5707-1F9A-4330-95DC-49144E20FABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1613033B-C478-42D4-BA16-1F05B12B4E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -337,15 +337,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -375,6 +375,174 @@
       </c>
       <c r="J1">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="J12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="J16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="J17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="J18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <v>24</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>26</v>
+      </c>
+      <c r="I19">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>